<commit_message>
graph in backend and x error
</commit_message>
<xml_diff>
--- a/backend/demand.xlsx
+++ b/backend/demand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinav/Downloads/hel/Supply-Chain-Optimization-Using-Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinav/Code/web-dev/codeutsava/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0FFD33-E6C3-174C-9090-5F88A1149D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517853FE-989A-D14A-B92D-72B64184EAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="8900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="4860" windowWidth="23040" windowHeight="8900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>2800000</v>
+        <v>904380</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>90000</v>
+        <v>823455</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>1700000</v>
+        <v>1345000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -480,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>145000</v>
+        <v>345700</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -488,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>160000</v>
+        <v>465000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>